<commit_message>
Solo falata ordenes de pedido
</commit_message>
<xml_diff>
--- a/NB.xlsx
+++ b/NB.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>PLAZO</t>
   </si>
@@ -48,6 +48,27 @@
     <t>P5</t>
   </si>
   <si>
+    <t>P6</t>
+  </si>
+  <si>
+    <t>P7</t>
+  </si>
+  <si>
+    <t>P8</t>
+  </si>
+  <si>
+    <t>P9</t>
+  </si>
+  <si>
+    <t>P10</t>
+  </si>
+  <si>
+    <t>P11</t>
+  </si>
+  <si>
+    <t>P12</t>
+  </si>
+  <si>
     <t>C1</t>
   </si>
   <si>
@@ -73,9 +94,6 @@
   </si>
   <si>
     <t>C3</t>
-  </si>
-  <si>
-    <t>C4</t>
   </si>
 </sst>
 </file>
@@ -120,7 +138,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -162,205 +180,294 @@
       <c r="J2" t="s">
         <v>10</v>
       </c>
+      <c r="K2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="C3" t="n">
         <v>0.0</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="n">
-        <v>140.0</v>
+        <v>19</v>
       </c>
       <c r="J3" t="n">
-        <v>50.0</v>
+        <v>200.0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>190.0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>200.0</v>
       </c>
     </row>
     <row r="4">
       <c r="E4" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="L4" t="n">
+        <v>201.0</v>
       </c>
     </row>
     <row r="5">
       <c r="E5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F5" t="n">
-        <f>B3</f>
+        <v>20.0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q5" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="6">
       <c r="E6" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="J6" t="n">
+        <v>180.0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>189.0</v>
       </c>
     </row>
     <row r="7">
       <c r="E7" t="s">
-        <v>16</v>
+        <v>23</v>
+      </c>
+      <c r="J7" t="n">
+        <v>180.0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>189.0</v>
       </c>
     </row>
     <row r="8">
       <c r="E8" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0</v>
+        <v>100.0</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10">
       <c r="E10" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11">
       <c r="E11" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F11" t="n">
-        <f>B9</f>
-        <v>0.0</v>
+        <v>100.0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="O11" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="P11" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>100.0</v>
       </c>
     </row>
     <row r="12">
       <c r="E12" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13">
       <c r="E13" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14">
       <c r="E14" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="B15" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="C15" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="D15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" t="s">
         <v>19</v>
-      </c>
-      <c r="E15" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="16">
       <c r="E16" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17">
       <c r="E17" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F17" t="n">
-        <f>B15</f>
-        <v>0.0</v>
+        <v>50.0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="M17" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="N17" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="O17" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="P17" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="18">
       <c r="E18" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19">
       <c r="E19" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20">
       <c r="E20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="B21" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="E22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="E23" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" t="n">
-        <f>B21</f>
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="E24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="E25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="E26" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="18">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F1:Q1"/>
     <mergeCell ref="A3:A8"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="C3:C8"/>
@@ -373,10 +480,6 @@
     <mergeCell ref="B15:B20"/>
     <mergeCell ref="C15:C20"/>
     <mergeCell ref="D15:D20"/>
-    <mergeCell ref="A21:A26"/>
-    <mergeCell ref="B21:B26"/>
-    <mergeCell ref="C21:C26"/>
-    <mergeCell ref="D21:D26"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Nivel 0 al 100
</commit_message>
<xml_diff>
--- a/NB.xlsx
+++ b/NB.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>PLAZO</t>
   </si>
@@ -46,27 +46,6 @@
   </si>
   <si>
     <t>P5</t>
-  </si>
-  <si>
-    <t>P6</t>
-  </si>
-  <si>
-    <t>P7</t>
-  </si>
-  <si>
-    <t>P8</t>
-  </si>
-  <si>
-    <t>P9</t>
-  </si>
-  <si>
-    <t>P10</t>
-  </si>
-  <si>
-    <t>P11</t>
-  </si>
-  <si>
-    <t>P12</t>
   </si>
   <si>
     <t>C1</t>
@@ -138,7 +117,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -180,284 +159,206 @@
       <c r="J2" t="s">
         <v>10</v>
       </c>
-      <c r="K2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O2" t="s">
-        <v>15</v>
-      </c>
-      <c r="P2" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="B3" t="n">
-        <v>20.0</v>
+        <v>1.0</v>
       </c>
       <c r="C3" t="n">
         <v>0.0</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>12</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>5.0</v>
       </c>
       <c r="J3" t="n">
-        <v>200.0</v>
-      </c>
-      <c r="L3" t="n">
-        <v>190.0</v>
-      </c>
-      <c r="M3" t="n">
-        <v>200.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="4">
       <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" t="n">
-        <v>201.0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5">
       <c r="E5" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F5" t="n">
-        <v>20.0</v>
+        <v>1.0</v>
       </c>
       <c r="G5" t="n">
-        <v>20.0</v>
+        <v>0.0</v>
       </c>
       <c r="H5" t="n">
-        <v>20.0</v>
+        <v>0.0</v>
       </c>
       <c r="I5" t="n">
-        <v>20.0</v>
+        <v>0.0</v>
       </c>
       <c r="J5" t="n">
-        <v>20.0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M5" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q5" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="6">
       <c r="E6" t="s">
-        <v>22</v>
+        <v>15</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>5.0</v>
       </c>
       <c r="J6" t="n">
-        <v>180.0</v>
-      </c>
-      <c r="M6" t="n">
-        <v>189.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="7">
       <c r="E7" t="s">
-        <v>23</v>
+        <v>16</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>5.0</v>
       </c>
       <c r="J7" t="n">
-        <v>180.0</v>
-      </c>
-      <c r="M7" t="n">
-        <v>189.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="8">
       <c r="E8" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="F8" t="n">
+        <v>7.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="B9" t="n">
-        <v>100.0</v>
+        <v>5.0</v>
       </c>
       <c r="C9" t="n">
         <v>1.0</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
       <c r="E10" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11">
       <c r="E11" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F11" t="n">
-        <v>100.0</v>
+        <v>5.0</v>
       </c>
       <c r="G11" t="n">
-        <v>100.0</v>
+        <v>5.0</v>
       </c>
       <c r="H11" t="n">
-        <v>100.0</v>
+        <v>5.0</v>
       </c>
       <c r="I11" t="n">
-        <v>100.0</v>
+        <v>5.0</v>
       </c>
       <c r="J11" t="n">
-        <v>100.0</v>
-      </c>
-      <c r="K11" t="n">
-        <v>100.0</v>
-      </c>
-      <c r="L11" t="n">
-        <v>100.0</v>
-      </c>
-      <c r="M11" t="n">
-        <v>100.0</v>
-      </c>
-      <c r="N11" t="n">
-        <v>100.0</v>
-      </c>
-      <c r="O11" t="n">
-        <v>100.0</v>
-      </c>
-      <c r="P11" t="n">
-        <v>100.0</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>100.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="12">
       <c r="E12" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13">
       <c r="E13" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14">
       <c r="E14" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="B15" t="n">
-        <v>50.0</v>
+        <v>5.0</v>
       </c>
       <c r="C15" t="n">
         <v>2.0</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E15" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16">
       <c r="E16" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17">
       <c r="E17" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F17" t="n">
-        <v>50.0</v>
+        <v>5.0</v>
       </c>
       <c r="G17" t="n">
-        <v>50.0</v>
+        <v>5.0</v>
       </c>
       <c r="H17" t="n">
-        <v>50.0</v>
+        <v>5.0</v>
       </c>
       <c r="I17" t="n">
-        <v>50.0</v>
+        <v>5.0</v>
       </c>
       <c r="J17" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="K17" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="L17" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="M17" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="N17" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="O17" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="P17" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="Q17" t="n">
-        <v>50.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="18">
       <c r="E18" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19">
       <c r="E19" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20">
       <c r="E20" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -467,7 +368,7 @@
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:Q1"/>
+    <mergeCell ref="F1:J1"/>
     <mergeCell ref="A3:A8"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="C3:C8"/>

</xml_diff>